<commit_message>
updated 'create_resonance_enchanted_book' advancement to trigger in more cases
</commit_message>
<xml_diff>
--- a/raw/Fluid_Interactions.xlsx
+++ b/raw/Fluid_Interactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863C8E62-80FD-43D0-AEC2-C6C1D607DF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C285D56-97D9-4AC5-A5DC-1E97231AF00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22890" yWindow="0" windowWidth="28710" windowHeight="21000" xr2:uid="{C062C883-C536-49F0-A3FB-1F783D9E299D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34395" windowHeight="21000" xr2:uid="{C062C883-C536-49F0-A3FB-1F783D9E299D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Water</t>
   </si>
@@ -100,6 +91,9 @@
   </si>
   <si>
     <t>Soul Sand / Soul Soil</t>
+  </si>
+  <si>
+    <t>Granite</t>
   </si>
 </sst>
 </file>
@@ -486,7 +480,7 @@
   <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +599,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
additional recipes & missing translation
</commit_message>
<xml_diff>
--- a/raw/Fluid_Interactions.xlsx
+++ b/raw/Fluid_Interactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C865A7D8-02FE-4C2A-9E52-89CA953E0C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D34BEC-D649-4B19-99FD-4CEBE1FCB1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{C062C883-C536-49F0-A3FB-1F783D9E299D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34395" windowHeight="21000" xr2:uid="{C062C883-C536-49F0-A3FB-1F783D9E299D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Water</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Slush</t>
+  </si>
+  <si>
+    <t>Dragonrot Dipping:</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398016E1-6FAD-49C3-B1B5-A6EC3CDF6D98}">
-  <dimension ref="B2:H17"/>
+  <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B12" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,32 +637,37 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>19</v>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>